<commit_message>
pushing the code to gibhhub
</commit_message>
<xml_diff>
--- a/CommonData/CommonD.xlsx
+++ b/CommonData/CommonD.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chill\sravan\Sdet\CommonData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chill\git\vtiger\Sdet\CommonData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8343FCD0-8F1C-4DD1-9CD6-C4253A8FB212}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92828A88-DD50-44C1-B156-BAE25B4B3EA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{827599DD-DEFD-4C0F-97ED-D8E8E8027F63}"/>
+    <workbookView xWindow="5196" yWindow="3132" windowWidth="17280" windowHeight="8880" xr2:uid="{827599DD-DEFD-4C0F-97ED-D8E8E8027F63}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="35">
   <si>
     <t>Mr.</t>
   </si>
@@ -127,6 +127,21 @@
   </si>
   <si>
     <t>Education</t>
+  </si>
+  <si>
+    <t>Testyantra</t>
+  </si>
+  <si>
+    <t>Yogendra</t>
+  </si>
+  <si>
+    <t>raja</t>
+  </si>
+  <si>
+    <t>nalla</t>
+  </si>
+  <si>
+    <t>Biotechnology</t>
   </si>
 </sst>
 </file>
@@ -490,10 +505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8168B26-3AE2-4527-B6C7-ABC41DDEB9BC}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -556,6 +571,33 @@
         <v>27</v>
       </c>
     </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" t="s">
+        <v>33</v>
+      </c>
+    </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>0</v>
@@ -573,6 +615,14 @@
         <v>2</v>
       </c>
       <c r="F11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>